<commit_message>
created ADC parts sheet
</commit_message>
<xml_diff>
--- a/MCU_Selection.xlsx
+++ b/MCU_Selection.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aae1ce134ce7b691/GaTech/PalmHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aae1ce134ce7b691/GaTech/PalmHub/Electrical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{91928F9B-5B07-490E-82FB-072828D7E6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1889789E-79D2-409D-8036-59CD93ED1A0F}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{91928F9B-5B07-490E-82FB-072828D7E6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C49FAF99-542F-4CE0-8544-0094FD63B67E}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Parts" sheetId="1" r:id="rId1"/>
-    <sheet name="README" sheetId="2" r:id="rId2"/>
+    <sheet name="Microcontroller" sheetId="1" r:id="rId1"/>
+    <sheet name="ADC" sheetId="3" r:id="rId2"/>
+    <sheet name="Readme" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>MCU</t>
   </si>
@@ -180,6 +179,63 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/microchip-technology/ATSAMD51J18A-AUT/7390301 </t>
+  </si>
+  <si>
+    <t>ATMega168p</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t># Chan</t>
+  </si>
+  <si>
+    <t>Sample Rate</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>Additional notes</t>
+  </si>
+  <si>
+    <t>ADC108S102</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Texas Inst</t>
+  </si>
+  <si>
+    <t>Res Bits</t>
+  </si>
+  <si>
+    <t>500k-1M</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>Price ($)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/texas-instruments/ADC108S102CIMT-NOPB/953338 </t>
+  </si>
+  <si>
+    <t>ADC128S102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/texas-instruments/ADC128S102CIMTX-NOPB/1870710 </t>
+  </si>
+  <si>
+    <t>ADS7955SDBT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/texas-instruments/ADS7955SDBT/1880865 </t>
+  </si>
+  <si>
+    <t>1M</t>
   </si>
 </sst>
 </file>
@@ -607,20 +663,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="14.5859375" customWidth="1"/>
-    <col min="2" max="2" width="17.46875" customWidth="1"/>
+    <col min="2" max="2" width="17.41015625" customWidth="1"/>
     <col min="6" max="6" width="9.5859375" customWidth="1"/>
-    <col min="7" max="7" width="13.8203125" customWidth="1"/>
-    <col min="8" max="8" width="11.3515625" customWidth="1"/>
-    <col min="10" max="10" width="8.9375" style="2"/>
-    <col min="11" max="11" width="11.05859375" customWidth="1"/>
-    <col min="12" max="12" width="12.64453125" customWidth="1"/>
+    <col min="7" max="7" width="13.87890625" customWidth="1"/>
+    <col min="8" max="8" width="11.29296875" customWidth="1"/>
+    <col min="10" max="10" width="9" style="2"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="12.703125" customWidth="1"/>
     <col min="13" max="13" width="54.703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -705,7 +761,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -963,7 +1019,7 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="K9">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>42</v>
@@ -1058,11 +1114,159 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2482C00-5892-4A51-A753-7A14F207963C}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="13.703125" customWidth="1"/>
+    <col min="2" max="2" width="11.17578125" customWidth="1"/>
+    <col min="5" max="5" width="10.87890625" customWidth="1"/>
+    <col min="7" max="7" width="8.9375" style="2"/>
+    <col min="8" max="8" width="14.17578125" customWidth="1"/>
+    <col min="9" max="9" width="13.52734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="2">
+        <v>8.33</v>
+      </c>
+      <c r="H2">
+        <v>173</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="2">
+        <v>8.33</v>
+      </c>
+      <c r="H3">
+        <v>3708</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="2">
+        <v>6.66</v>
+      </c>
+      <c r="H4">
+        <v>422</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{0865EFFA-70F6-4820-9A8B-61650BD7CDBF}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{1D6417FC-36E3-4D54-BEFC-65162E8EA072}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{DD8EF9F4-B090-4C32-A38E-D964DA7D5300}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474C3C1E-BDCB-452A-811E-B60AAE3916EF}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Transfer palm hub ADC schematic
</commit_message>
<xml_diff>
--- a/MCU_Selection.xlsx
+++ b/MCU_Selection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aniketh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aniketh\Documents\GitHub\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBEB444-D635-4A1E-9CE5-70E8EC8082FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015877D8-BBDA-4878-8E48-F9FAB1EE6066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1341,7 +1341,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1557,7 +1557,7 @@
       <c r="H8" t="s">
         <v>85</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1586,7 +1586,7 @@
       <c r="H9">
         <v>1828</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1615,7 +1615,7 @@
       <c r="H10">
         <v>71225</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1654,9 +1654,12 @@
     <hyperlink ref="I3" r:id="rId2" xr:uid="{B9847A50-2847-4E5A-BCD4-3165F4E1A03D}"/>
     <hyperlink ref="I4" r:id="rId3" xr:uid="{D81286FC-0955-4FD0-AB04-0DA136BF7FBE}"/>
     <hyperlink ref="I11" r:id="rId4" xr:uid="{0BEB995F-D31A-4D34-8922-165010B26DCC}"/>
+    <hyperlink ref="I8" r:id="rId5" xr:uid="{717A0E9D-F41D-431D-A2CD-6298CECBD464}"/>
+    <hyperlink ref="I9" r:id="rId6" xr:uid="{FF37342D-93F9-4AEF-9F61-41FF6E583A39}"/>
+    <hyperlink ref="I10" r:id="rId7" xr:uid="{1A6FF771-5E2C-4089-B371-6876D16BAC58}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>